<commit_message>
Update RESULTS ScenariosBenefit Street AS IS.xlsx
</commit_message>
<xml_diff>
--- a/outputs/RESULTS ScenariosBenefit Street AS IS.xlsx
+++ b/outputs/RESULTS ScenariosBenefit Street AS IS.xlsx
@@ -31,508 +31,508 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
-    <t>[3.99-4.141]</t>
-  </si>
-  <si>
-    <t>[4.141-4.293]</t>
-  </si>
-  <si>
-    <t>[4.293-4.445]</t>
-  </si>
-  <si>
-    <t>[4.445-4.597]</t>
-  </si>
-  <si>
-    <t>[4.597-4.749]</t>
-  </si>
-  <si>
-    <t>[4.749-4.9]</t>
-  </si>
-  <si>
-    <t>[4.9-5.052]</t>
-  </si>
-  <si>
-    <t>[5.052-5.204]</t>
-  </si>
-  <si>
-    <t>[5.204-5.356]</t>
-  </si>
-  <si>
-    <t>[5.356-5.507]</t>
-  </si>
-  <si>
-    <t>[5.507-5.659]</t>
-  </si>
-  <si>
-    <t>[5.659-5.811]</t>
-  </si>
-  <si>
-    <t>[5.811-5.963]</t>
-  </si>
-  <si>
-    <t>[5.963-6.115]</t>
-  </si>
-  <si>
-    <t>[4.157-4.27]</t>
-  </si>
-  <si>
-    <t>[4.27-4.383]</t>
-  </si>
-  <si>
-    <t>[4.383-4.496]</t>
-  </si>
-  <si>
-    <t>[4.496-4.608]</t>
-  </si>
-  <si>
-    <t>[4.608-4.721]</t>
-  </si>
-  <si>
-    <t>[4.721-4.834]</t>
-  </si>
-  <si>
-    <t>[4.834-4.947]</t>
-  </si>
-  <si>
-    <t>[4.947-5.059]</t>
-  </si>
-  <si>
-    <t>[5.059-5.172]</t>
-  </si>
-  <si>
-    <t>[5.172-5.285]</t>
-  </si>
-  <si>
-    <t>[5.285-5.398]</t>
-  </si>
-  <si>
-    <t>[5.398-5.51]</t>
-  </si>
-  <si>
-    <t>[5.51-5.623]</t>
-  </si>
-  <si>
-    <t>[5.623-5.736]</t>
-  </si>
-  <si>
-    <t>[4.469-4.587]</t>
-  </si>
-  <si>
-    <t>[4.587-4.704]</t>
-  </si>
-  <si>
-    <t>[4.704-4.822]</t>
-  </si>
-  <si>
-    <t>[4.822-4.939]</t>
-  </si>
-  <si>
-    <t>[4.939-5.057]</t>
-  </si>
-  <si>
-    <t>[5.057-5.174]</t>
-  </si>
-  <si>
-    <t>[5.174-5.292]</t>
-  </si>
-  <si>
-    <t>[5.292-5.409]</t>
-  </si>
-  <si>
-    <t>[5.409-5.527]</t>
-  </si>
-  <si>
-    <t>[5.527-5.644]</t>
-  </si>
-  <si>
-    <t>[5.644-5.762]</t>
-  </si>
-  <si>
-    <t>[5.762-5.88]</t>
-  </si>
-  <si>
-    <t>[5.88-5.997]</t>
-  </si>
-  <si>
-    <t>[5.997-6.115]</t>
-  </si>
-  <si>
-    <t>[3.99-4.113]</t>
-  </si>
-  <si>
-    <t>[4.113-4.236]</t>
-  </si>
-  <si>
-    <t>[4.236-4.359]</t>
-  </si>
-  <si>
-    <t>[4.359-4.483]</t>
-  </si>
-  <si>
-    <t>[4.483-4.606]</t>
-  </si>
-  <si>
-    <t>[4.606-4.729]</t>
-  </si>
-  <si>
-    <t>[4.729-4.852]</t>
-  </si>
-  <si>
-    <t>[4.852-4.976]</t>
-  </si>
-  <si>
-    <t>[4.976-5.099]</t>
-  </si>
-  <si>
-    <t>[5.099-5.222]</t>
-  </si>
-  <si>
-    <t>[5.222-5.345]</t>
-  </si>
-  <si>
-    <t>[5.345-5.469]</t>
-  </si>
-  <si>
-    <t>[5.469-5.592]</t>
-  </si>
-  <si>
-    <t>[5.592-5.715]</t>
-  </si>
-  <si>
-    <t>[8.22-8.48]</t>
-  </si>
-  <si>
-    <t>[8.48-8.74]</t>
-  </si>
-  <si>
-    <t>[8.74-9.0]</t>
-  </si>
-  <si>
-    <t>[9.0-9.26]</t>
-  </si>
-  <si>
-    <t>[9.26-9.53]</t>
-  </si>
-  <si>
-    <t>[9.53-9.79]</t>
-  </si>
-  <si>
-    <t>[9.79-10.05]</t>
-  </si>
-  <si>
-    <t>[10.05-10.31]</t>
-  </si>
-  <si>
-    <t>[10.31-10.57]</t>
-  </si>
-  <si>
-    <t>[10.57-10.83]</t>
-  </si>
-  <si>
-    <t>[10.83-11.09]</t>
-  </si>
-  <si>
-    <t>[11.09-11.36]</t>
-  </si>
-  <si>
-    <t>[11.36-11.62]</t>
-  </si>
-  <si>
-    <t>[11.62-11.88]</t>
-  </si>
-  <si>
-    <t>[8.89-9.09]</t>
-  </si>
-  <si>
-    <t>[9.09-9.28]</t>
-  </si>
-  <si>
-    <t>[9.28-9.47]</t>
-  </si>
-  <si>
-    <t>[9.47-9.67]</t>
-  </si>
-  <si>
-    <t>[9.67-9.86]</t>
-  </si>
-  <si>
-    <t>[9.86-10.06]</t>
-  </si>
-  <si>
-    <t>[10.06-10.25]</t>
-  </si>
-  <si>
-    <t>[10.25-10.44]</t>
-  </si>
-  <si>
-    <t>[10.44-10.64]</t>
-  </si>
-  <si>
-    <t>[10.64-10.83]</t>
-  </si>
-  <si>
-    <t>[10.83-11.03]</t>
-  </si>
-  <si>
-    <t>[11.03-11.22]</t>
-  </si>
-  <si>
-    <t>[11.22-11.41]</t>
-  </si>
-  <si>
-    <t>[11.41-11.61]</t>
-  </si>
-  <si>
-    <t>[8.22-8.42]</t>
-  </si>
-  <si>
-    <t>[8.42-8.62]</t>
-  </si>
-  <si>
-    <t>[8.62-8.83]</t>
-  </si>
-  <si>
-    <t>[8.83-9.03]</t>
-  </si>
-  <si>
-    <t>[9.03-9.23]</t>
-  </si>
-  <si>
-    <t>[9.23-9.43]</t>
-  </si>
-  <si>
-    <t>[9.43-9.64]</t>
-  </si>
-  <si>
-    <t>[9.64-9.84]</t>
-  </si>
-  <si>
-    <t>[9.84-10.04]</t>
-  </si>
-  <si>
-    <t>[10.04-10.24]</t>
-  </si>
-  <si>
-    <t>[10.24-10.45]</t>
-  </si>
-  <si>
-    <t>[10.45-10.65]</t>
-  </si>
-  <si>
-    <t>[10.65-10.85]</t>
-  </si>
-  <si>
-    <t>[10.85-11.05]</t>
-  </si>
-  <si>
-    <t>[8.93-9.14]</t>
-  </si>
-  <si>
-    <t>[9.14-9.35]</t>
-  </si>
-  <si>
-    <t>[9.35-9.56]</t>
-  </si>
-  <si>
-    <t>[9.56-9.77]</t>
-  </si>
-  <si>
-    <t>[9.77-9.98]</t>
-  </si>
-  <si>
-    <t>[9.98-10.19]</t>
-  </si>
-  <si>
-    <t>[10.19-10.4]</t>
-  </si>
-  <si>
-    <t>[10.4-10.61]</t>
-  </si>
-  <si>
-    <t>[10.61-10.82]</t>
-  </si>
-  <si>
-    <t>[10.82-11.04]</t>
-  </si>
-  <si>
-    <t>[11.04-11.25]</t>
-  </si>
-  <si>
-    <t>[11.25-11.46]</t>
-  </si>
-  <si>
-    <t>[11.46-11.67]</t>
-  </si>
-  <si>
-    <t>[11.67-11.88]</t>
-  </si>
-  <si>
-    <t>[47.83-48.55]</t>
-  </si>
-  <si>
-    <t>[48.55-49.27]</t>
-  </si>
-  <si>
-    <t>[49.27-50.0]</t>
-  </si>
-  <si>
-    <t>[50.0-50.72]</t>
-  </si>
-  <si>
-    <t>[50.72-51.44]</t>
-  </si>
-  <si>
-    <t>[51.44-52.16]</t>
-  </si>
-  <si>
-    <t>[52.16-52.88]</t>
-  </si>
-  <si>
-    <t>[52.88-53.6]</t>
-  </si>
-  <si>
-    <t>[53.6-54.32]</t>
-  </si>
-  <si>
-    <t>[54.32-55.04]</t>
-  </si>
-  <si>
-    <t>[55.04-55.76]</t>
-  </si>
-  <si>
-    <t>[55.76-56.49]</t>
-  </si>
-  <si>
-    <t>[56.49-57.21]</t>
-  </si>
-  <si>
-    <t>[57.21-57.93]</t>
-  </si>
-  <si>
-    <t>[48.55-49.15]</t>
-  </si>
-  <si>
-    <t>[49.15-49.74]</t>
-  </si>
-  <si>
-    <t>[49.74-50.33]</t>
-  </si>
-  <si>
-    <t>[50.33-50.92]</t>
-  </si>
-  <si>
-    <t>[50.92-51.51]</t>
-  </si>
-  <si>
-    <t>[51.51-52.11]</t>
-  </si>
-  <si>
-    <t>[52.11-52.7]</t>
-  </si>
-  <si>
-    <t>[52.7-53.29]</t>
-  </si>
-  <si>
-    <t>[53.29-53.88]</t>
-  </si>
-  <si>
-    <t>[53.88-54.47]</t>
-  </si>
-  <si>
-    <t>[54.47-55.07]</t>
-  </si>
-  <si>
-    <t>[55.07-55.66]</t>
-  </si>
-  <si>
-    <t>[55.66-56.25]</t>
-  </si>
-  <si>
-    <t>[56.25-56.84]</t>
-  </si>
-  <si>
-    <t>[47.83-48.43]</t>
-  </si>
-  <si>
-    <t>[48.43-49.03]</t>
-  </si>
-  <si>
-    <t>[49.03-49.63]</t>
-  </si>
-  <si>
-    <t>[49.63-50.22]</t>
-  </si>
-  <si>
-    <t>[50.22-50.82]</t>
-  </si>
-  <si>
-    <t>[50.82-51.42]</t>
-  </si>
-  <si>
-    <t>[51.42-52.02]</t>
-  </si>
-  <si>
-    <t>[52.02-52.62]</t>
-  </si>
-  <si>
-    <t>[52.62-53.22]</t>
-  </si>
-  <si>
-    <t>[53.22-53.81]</t>
-  </si>
-  <si>
-    <t>[53.81-54.41]</t>
-  </si>
-  <si>
-    <t>[54.41-55.01]</t>
-  </si>
-  <si>
-    <t>[55.01-55.61]</t>
-  </si>
-  <si>
-    <t>[55.61-56.21]</t>
-  </si>
-  <si>
-    <t>[50.0-50.57]</t>
-  </si>
-  <si>
-    <t>[50.57-51.14]</t>
-  </si>
-  <si>
-    <t>[51.14-51.7]</t>
-  </si>
-  <si>
-    <t>[51.7-52.27]</t>
-  </si>
-  <si>
-    <t>[52.27-52.83]</t>
-  </si>
-  <si>
-    <t>[52.83-53.4]</t>
-  </si>
-  <si>
-    <t>[53.4-53.97]</t>
-  </si>
-  <si>
-    <t>[53.97-54.53]</t>
-  </si>
-  <si>
-    <t>[54.53-55.1]</t>
-  </si>
-  <si>
-    <t>[55.1-55.66]</t>
-  </si>
-  <si>
-    <t>[55.66-56.23]</t>
-  </si>
-  <si>
-    <t>[56.23-56.8]</t>
-  </si>
-  <si>
-    <t>[56.8-57.36]</t>
-  </si>
-  <si>
-    <t>[57.36-57.93]</t>
+    <t>[3.935-4.098]</t>
+  </si>
+  <si>
+    <t>[4.098-4.262]</t>
+  </si>
+  <si>
+    <t>[4.262-4.425]</t>
+  </si>
+  <si>
+    <t>[4.425-4.589]</t>
+  </si>
+  <si>
+    <t>[4.589-4.752]</t>
+  </si>
+  <si>
+    <t>[4.752-4.916]</t>
+  </si>
+  <si>
+    <t>[4.916-5.079]</t>
+  </si>
+  <si>
+    <t>[5.079-5.243]</t>
+  </si>
+  <si>
+    <t>[5.243-5.406]</t>
+  </si>
+  <si>
+    <t>[5.406-5.57]</t>
+  </si>
+  <si>
+    <t>[5.57-5.733]</t>
+  </si>
+  <si>
+    <t>[5.733-5.897]</t>
+  </si>
+  <si>
+    <t>[5.897-6.06]</t>
+  </si>
+  <si>
+    <t>[6.06-6.224]</t>
+  </si>
+  <si>
+    <t>[4.142-4.277]</t>
+  </si>
+  <si>
+    <t>[4.277-4.412]</t>
+  </si>
+  <si>
+    <t>[4.412-4.546]</t>
+  </si>
+  <si>
+    <t>[4.546-4.681]</t>
+  </si>
+  <si>
+    <t>[4.681-4.816]</t>
+  </si>
+  <si>
+    <t>[4.816-4.951]</t>
+  </si>
+  <si>
+    <t>[4.951-5.086]</t>
+  </si>
+  <si>
+    <t>[5.086-5.221]</t>
+  </si>
+  <si>
+    <t>[5.221-5.356]</t>
+  </si>
+  <si>
+    <t>[5.356-5.491]</t>
+  </si>
+  <si>
+    <t>[5.491-5.626]</t>
+  </si>
+  <si>
+    <t>[5.626-5.761]</t>
+  </si>
+  <si>
+    <t>[5.761-5.896]</t>
+  </si>
+  <si>
+    <t>[5.896-6.031]</t>
+  </si>
+  <si>
+    <t>[4.299-4.437]</t>
+  </si>
+  <si>
+    <t>[4.437-4.574]</t>
+  </si>
+  <si>
+    <t>[4.574-4.711]</t>
+  </si>
+  <si>
+    <t>[4.711-4.849]</t>
+  </si>
+  <si>
+    <t>[4.849-4.986]</t>
+  </si>
+  <si>
+    <t>[4.986-5.124]</t>
+  </si>
+  <si>
+    <t>[5.124-5.261]</t>
+  </si>
+  <si>
+    <t>[5.261-5.399]</t>
+  </si>
+  <si>
+    <t>[5.399-5.536]</t>
+  </si>
+  <si>
+    <t>[5.536-5.674]</t>
+  </si>
+  <si>
+    <t>[5.674-5.811]</t>
+  </si>
+  <si>
+    <t>[5.811-5.949]</t>
+  </si>
+  <si>
+    <t>[5.949-6.086]</t>
+  </si>
+  <si>
+    <t>[6.086-6.224]</t>
+  </si>
+  <si>
+    <t>[3.935-4.044]</t>
+  </si>
+  <si>
+    <t>[4.044-4.154]</t>
+  </si>
+  <si>
+    <t>[4.154-4.263]</t>
+  </si>
+  <si>
+    <t>[4.263-4.373]</t>
+  </si>
+  <si>
+    <t>[4.373-4.483]</t>
+  </si>
+  <si>
+    <t>[4.483-4.592]</t>
+  </si>
+  <si>
+    <t>[4.592-4.702]</t>
+  </si>
+  <si>
+    <t>[4.702-4.811]</t>
+  </si>
+  <si>
+    <t>[4.811-4.921]</t>
+  </si>
+  <si>
+    <t>[4.921-5.03]</t>
+  </si>
+  <si>
+    <t>[5.03-5.14]</t>
+  </si>
+  <si>
+    <t>[5.14-5.249]</t>
+  </si>
+  <si>
+    <t>[5.249-5.359]</t>
+  </si>
+  <si>
+    <t>[5.359-5.468]</t>
+  </si>
+  <si>
+    <t>[8.02-8.31]</t>
+  </si>
+  <si>
+    <t>[8.31-8.59]</t>
+  </si>
+  <si>
+    <t>[8.59-8.87]</t>
+  </si>
+  <si>
+    <t>[8.87-9.15]</t>
+  </si>
+  <si>
+    <t>[9.15-9.44]</t>
+  </si>
+  <si>
+    <t>[9.44-9.72]</t>
+  </si>
+  <si>
+    <t>[9.72-10.0]</t>
+  </si>
+  <si>
+    <t>[10.0-10.28]</t>
+  </si>
+  <si>
+    <t>[10.28-10.56]</t>
+  </si>
+  <si>
+    <t>[10.56-10.85]</t>
+  </si>
+  <si>
+    <t>[10.85-11.13]</t>
+  </si>
+  <si>
+    <t>[11.13-11.41]</t>
+  </si>
+  <si>
+    <t>[11.41-11.69]</t>
+  </si>
+  <si>
+    <t>[11.69-11.98]</t>
+  </si>
+  <si>
+    <t>[8.37-8.6]</t>
+  </si>
+  <si>
+    <t>[8.6-8.83]</t>
+  </si>
+  <si>
+    <t>[8.83-9.06]</t>
+  </si>
+  <si>
+    <t>[9.06-9.29]</t>
+  </si>
+  <si>
+    <t>[9.29-9.53]</t>
+  </si>
+  <si>
+    <t>[9.53-9.76]</t>
+  </si>
+  <si>
+    <t>[9.76-9.99]</t>
+  </si>
+  <si>
+    <t>[9.99-10.22]</t>
+  </si>
+  <si>
+    <t>[10.22-10.45]</t>
+  </si>
+  <si>
+    <t>[10.45-10.69]</t>
+  </si>
+  <si>
+    <t>[10.69-10.92]</t>
+  </si>
+  <si>
+    <t>[10.92-11.15]</t>
+  </si>
+  <si>
+    <t>[11.15-11.38]</t>
+  </si>
+  <si>
+    <t>[11.38-11.61]</t>
+  </si>
+  <si>
+    <t>[8.02-8.26]</t>
+  </si>
+  <si>
+    <t>[8.26-8.5]</t>
+  </si>
+  <si>
+    <t>[8.5-8.74]</t>
+  </si>
+  <si>
+    <t>[8.74-8.98]</t>
+  </si>
+  <si>
+    <t>[8.98-9.22]</t>
+  </si>
+  <si>
+    <t>[9.22-9.46]</t>
+  </si>
+  <si>
+    <t>[9.46-9.69]</t>
+  </si>
+  <si>
+    <t>[9.69-9.93]</t>
+  </si>
+  <si>
+    <t>[9.93-10.17]</t>
+  </si>
+  <si>
+    <t>[10.17-10.41]</t>
+  </si>
+  <si>
+    <t>[10.41-10.65]</t>
+  </si>
+  <si>
+    <t>[10.65-10.89]</t>
+  </si>
+  <si>
+    <t>[10.89-11.13]</t>
+  </si>
+  <si>
+    <t>[11.13-11.36]</t>
+  </si>
+  <si>
+    <t>[9.37-9.55]</t>
+  </si>
+  <si>
+    <t>[9.55-9.74]</t>
+  </si>
+  <si>
+    <t>[9.74-9.93]</t>
+  </si>
+  <si>
+    <t>[9.93-10.11]</t>
+  </si>
+  <si>
+    <t>[10.11-10.3]</t>
+  </si>
+  <si>
+    <t>[10.3-10.48]</t>
+  </si>
+  <si>
+    <t>[10.48-10.67]</t>
+  </si>
+  <si>
+    <t>[10.67-10.86]</t>
+  </si>
+  <si>
+    <t>[10.86-11.04]</t>
+  </si>
+  <si>
+    <t>[11.04-11.23]</t>
+  </si>
+  <si>
+    <t>[11.23-11.42]</t>
+  </si>
+  <si>
+    <t>[11.42-11.6]</t>
+  </si>
+  <si>
+    <t>[11.6-11.79]</t>
+  </si>
+  <si>
+    <t>[11.79-11.98]</t>
+  </si>
+  <si>
+    <t>[48.56-49.23]</t>
+  </si>
+  <si>
+    <t>[49.23-49.89]</t>
+  </si>
+  <si>
+    <t>[49.89-50.55]</t>
+  </si>
+  <si>
+    <t>[50.55-51.22]</t>
+  </si>
+  <si>
+    <t>[51.22-51.88]</t>
+  </si>
+  <si>
+    <t>[51.88-52.55]</t>
+  </si>
+  <si>
+    <t>[52.55-53.21]</t>
+  </si>
+  <si>
+    <t>[53.21-53.88]</t>
+  </si>
+  <si>
+    <t>[53.88-54.54]</t>
+  </si>
+  <si>
+    <t>[54.54-55.2]</t>
+  </si>
+  <si>
+    <t>[55.2-55.87]</t>
+  </si>
+  <si>
+    <t>[55.87-56.53]</t>
+  </si>
+  <si>
+    <t>[56.53-57.2]</t>
+  </si>
+  <si>
+    <t>[57.2-57.86]</t>
+  </si>
+  <si>
+    <t>[49.18-49.74]</t>
+  </si>
+  <si>
+    <t>[49.74-50.29]</t>
+  </si>
+  <si>
+    <t>[50.29-50.85]</t>
+  </si>
+  <si>
+    <t>[50.85-51.41]</t>
+  </si>
+  <si>
+    <t>[51.41-51.96]</t>
+  </si>
+  <si>
+    <t>[51.96-52.52]</t>
+  </si>
+  <si>
+    <t>[52.52-53.08]</t>
+  </si>
+  <si>
+    <t>[53.08-53.63]</t>
+  </si>
+  <si>
+    <t>[53.63-54.19]</t>
+  </si>
+  <si>
+    <t>[54.19-54.75]</t>
+  </si>
+  <si>
+    <t>[54.75-55.3]</t>
+  </si>
+  <si>
+    <t>[55.3-55.86]</t>
+  </si>
+  <si>
+    <t>[55.86-56.42]</t>
+  </si>
+  <si>
+    <t>[56.42-56.97]</t>
+  </si>
+  <si>
+    <t>[48.56-49.18]</t>
+  </si>
+  <si>
+    <t>[49.18-49.79]</t>
+  </si>
+  <si>
+    <t>[49.79-50.4]</t>
+  </si>
+  <si>
+    <t>[50.4-51.02]</t>
+  </si>
+  <si>
+    <t>[51.02-51.63]</t>
+  </si>
+  <si>
+    <t>[51.63-52.25]</t>
+  </si>
+  <si>
+    <t>[52.25-52.86]</t>
+  </si>
+  <si>
+    <t>[52.86-53.47]</t>
+  </si>
+  <si>
+    <t>[53.47-54.09]</t>
+  </si>
+  <si>
+    <t>[54.09-54.7]</t>
+  </si>
+  <si>
+    <t>[54.7-55.32]</t>
+  </si>
+  <si>
+    <t>[55.32-55.93]</t>
+  </si>
+  <si>
+    <t>[55.93-56.54]</t>
+  </si>
+  <si>
+    <t>[56.54-57.16]</t>
+  </si>
+  <si>
+    <t>[49.9-50.47]</t>
+  </si>
+  <si>
+    <t>[50.47-51.04]</t>
+  </si>
+  <si>
+    <t>[51.04-51.61]</t>
+  </si>
+  <si>
+    <t>[51.61-52.18]</t>
+  </si>
+  <si>
+    <t>[52.18-52.75]</t>
+  </si>
+  <si>
+    <t>[52.75-53.31]</t>
+  </si>
+  <si>
+    <t>[53.31-53.88]</t>
+  </si>
+  <si>
+    <t>[53.88-54.45]</t>
+  </si>
+  <si>
+    <t>[54.45-55.02]</t>
+  </si>
+  <si>
+    <t>[55.02-55.59]</t>
+  </si>
+  <si>
+    <t>[55.59-56.16]</t>
+  </si>
+  <si>
+    <t>[56.16-56.73]</t>
+  </si>
+  <si>
+    <t>[56.73-57.29]</t>
+  </si>
+  <si>
+    <t>[57.29-57.86]</t>
   </si>
 </sst>
 </file>
@@ -674,25 +674,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>109</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>89</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -825,46 +825,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[8.89-9.09]</c:v>
+                  <c:v>[8.37-8.6]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[9.09-9.28]</c:v>
+                  <c:v>[8.6-8.83]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[9.28-9.47]</c:v>
+                  <c:v>[8.83-9.06]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[9.47-9.67]</c:v>
+                  <c:v>[9.06-9.29]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[9.67-9.86]</c:v>
+                  <c:v>[9.29-9.53]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[9.86-10.06]</c:v>
+                  <c:v>[9.53-9.76]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[10.06-10.25]</c:v>
+                  <c:v>[9.76-9.99]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[10.25-10.44]</c:v>
+                  <c:v>[9.99-10.22]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[10.44-10.64]</c:v>
+                  <c:v>[10.22-10.45]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[10.64-10.83]</c:v>
+                  <c:v>[10.45-10.69]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[10.83-11.03]</c:v>
+                  <c:v>[10.69-10.92]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[11.03-11.22]</c:v>
+                  <c:v>[10.92-11.15]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[11.22-11.41]</c:v>
+                  <c:v>[11.15-11.38]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.41-11.61]</c:v>
+                  <c:v>[11.38-11.61]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -876,46 +876,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>12</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1052,46 +1052,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[8.22-8.42]</c:v>
+                  <c:v>[8.02-8.26]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[8.42-8.62]</c:v>
+                  <c:v>[8.26-8.5]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[8.62-8.83]</c:v>
+                  <c:v>[8.5-8.74]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[8.83-9.03]</c:v>
+                  <c:v>[8.74-8.98]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[9.03-9.23]</c:v>
+                  <c:v>[8.98-9.22]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[9.23-9.43]</c:v>
+                  <c:v>[9.22-9.46]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[9.43-9.64]</c:v>
+                  <c:v>[9.46-9.69]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[9.64-9.84]</c:v>
+                  <c:v>[9.69-9.93]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[9.84-10.04]</c:v>
+                  <c:v>[9.93-10.17]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[10.04-10.24]</c:v>
+                  <c:v>[10.17-10.41]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[10.24-10.45]</c:v>
+                  <c:v>[10.41-10.65]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[10.45-10.65]</c:v>
+                  <c:v>[10.65-10.89]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[10.65-10.85]</c:v>
+                  <c:v>[10.89-11.13]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[10.85-11.05]</c:v>
+                  <c:v>[11.13-11.36]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1106,43 +1106,43 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13</c:v>
-                </c:pt>
                 <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1279,46 +1279,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[8.93-9.14]</c:v>
+                  <c:v>[9.37-9.55]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[9.14-9.35]</c:v>
+                  <c:v>[9.55-9.74]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[9.35-9.56]</c:v>
+                  <c:v>[9.74-9.93]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[9.56-9.77]</c:v>
+                  <c:v>[9.93-10.11]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[9.77-9.98]</c:v>
+                  <c:v>[10.11-10.3]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[9.98-10.19]</c:v>
+                  <c:v>[10.3-10.48]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[10.19-10.4]</c:v>
+                  <c:v>[10.48-10.67]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[10.4-10.61]</c:v>
+                  <c:v>[10.67-10.86]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[10.61-10.82]</c:v>
+                  <c:v>[10.86-11.04]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[10.82-11.04]</c:v>
+                  <c:v>[11.04-11.23]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[11.04-11.25]</c:v>
+                  <c:v>[11.23-11.42]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[11.25-11.46]</c:v>
+                  <c:v>[11.42-11.6]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[11.46-11.67]</c:v>
+                  <c:v>[11.6-11.79]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.67-11.88]</c:v>
+                  <c:v>[11.79-11.98]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1330,46 +1330,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1506,46 +1506,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[47.83-48.55]</c:v>
+                  <c:v>[48.56-49.23]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[48.55-49.27]</c:v>
+                  <c:v>[49.23-49.89]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[49.27-50.0]</c:v>
+                  <c:v>[49.89-50.55]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[50.0-50.72]</c:v>
+                  <c:v>[50.55-51.22]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[50.72-51.44]</c:v>
+                  <c:v>[51.22-51.88]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[51.44-52.16]</c:v>
+                  <c:v>[51.88-52.55]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[52.16-52.88]</c:v>
+                  <c:v>[52.55-53.21]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[52.88-53.6]</c:v>
+                  <c:v>[53.21-53.88]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[53.6-54.32]</c:v>
+                  <c:v>[53.88-54.54]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[54.32-55.04]</c:v>
+                  <c:v>[54.54-55.2]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[55.04-55.76]</c:v>
+                  <c:v>[55.2-55.87]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[55.76-56.49]</c:v>
+                  <c:v>[55.87-56.53]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[56.49-57.21]</c:v>
+                  <c:v>[56.53-57.2]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[57.21-57.93]</c:v>
+                  <c:v>[57.2-57.86]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1560,43 +1560,43 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1733,46 +1733,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[48.55-49.15]</c:v>
+                  <c:v>[49.18-49.74]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[49.15-49.74]</c:v>
+                  <c:v>[49.74-50.29]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[49.74-50.33]</c:v>
+                  <c:v>[50.29-50.85]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[50.33-50.92]</c:v>
+                  <c:v>[50.85-51.41]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[50.92-51.51]</c:v>
+                  <c:v>[51.41-51.96]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[51.51-52.11]</c:v>
+                  <c:v>[51.96-52.52]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[52.11-52.7]</c:v>
+                  <c:v>[52.52-53.08]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[52.7-53.29]</c:v>
+                  <c:v>[53.08-53.63]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[53.29-53.88]</c:v>
+                  <c:v>[53.63-54.19]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[53.88-54.47]</c:v>
+                  <c:v>[54.19-54.75]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[54.47-55.07]</c:v>
+                  <c:v>[54.75-55.3]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[55.07-55.66]</c:v>
+                  <c:v>[55.3-55.86]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[55.66-56.25]</c:v>
+                  <c:v>[55.86-56.42]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[56.25-56.84]</c:v>
+                  <c:v>[56.42-56.97]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1784,22 +1784,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>13</c:v>
@@ -1808,22 +1808,22 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1960,46 +1960,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[47.83-48.43]</c:v>
+                  <c:v>[48.56-49.18]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[48.43-49.03]</c:v>
+                  <c:v>[49.18-49.79]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[49.03-49.63]</c:v>
+                  <c:v>[49.79-50.4]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[49.63-50.22]</c:v>
+                  <c:v>[50.4-51.02]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[50.22-50.82]</c:v>
+                  <c:v>[51.02-51.63]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[50.82-51.42]</c:v>
+                  <c:v>[51.63-52.25]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[51.42-52.02]</c:v>
+                  <c:v>[52.25-52.86]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[52.02-52.62]</c:v>
+                  <c:v>[52.86-53.47]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[52.62-53.22]</c:v>
+                  <c:v>[53.47-54.09]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[53.22-53.81]</c:v>
+                  <c:v>[54.09-54.7]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[53.81-54.41]</c:v>
+                  <c:v>[54.7-55.32]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[54.41-55.01]</c:v>
+                  <c:v>[55.32-55.93]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[55.01-55.61]</c:v>
+                  <c:v>[55.93-56.54]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[55.61-56.21]</c:v>
+                  <c:v>[56.54-57.16]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2011,46 +2011,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2187,46 +2187,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[50.0-50.57]</c:v>
+                  <c:v>[49.9-50.47]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[50.57-51.14]</c:v>
+                  <c:v>[50.47-51.04]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[51.14-51.7]</c:v>
+                  <c:v>[51.04-51.61]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[51.7-52.27]</c:v>
+                  <c:v>[51.61-52.18]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[52.27-52.83]</c:v>
+                  <c:v>[52.18-52.75]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[52.83-53.4]</c:v>
+                  <c:v>[52.75-53.31]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[53.4-53.97]</c:v>
+                  <c:v>[53.31-53.88]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[53.97-54.53]</c:v>
+                  <c:v>[53.88-54.45]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[54.53-55.1]</c:v>
+                  <c:v>[54.45-55.02]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[55.1-55.66]</c:v>
+                  <c:v>[55.02-55.59]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[55.66-56.23]</c:v>
+                  <c:v>[55.59-56.16]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[56.23-56.8]</c:v>
+                  <c:v>[56.16-56.73]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[56.8-57.36]</c:v>
+                  <c:v>[56.73-57.29]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[57.36-57.93]</c:v>
+                  <c:v>[57.29-57.86]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2238,43 +2238,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>7</c:v>
-                </c:pt>
                 <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
@@ -2427,19 +2427,19 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2451,31 +2451,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2642,16 +2642,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2660,10 +2660,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2827,31 +2827,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2978,46 +2978,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.99-4.141]</c:v>
+                  <c:v>[3.935-4.098]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[4.141-4.293]</c:v>
+                  <c:v>[4.098-4.262]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[4.293-4.445]</c:v>
+                  <c:v>[4.262-4.425]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[4.445-4.597]</c:v>
+                  <c:v>[4.425-4.589]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[4.597-4.749]</c:v>
+                  <c:v>[4.589-4.752]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[4.749-4.9]</c:v>
+                  <c:v>[4.752-4.916]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[4.9-5.052]</c:v>
+                  <c:v>[4.916-5.079]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[5.052-5.204]</c:v>
+                  <c:v>[5.079-5.243]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[5.204-5.356]</c:v>
+                  <c:v>[5.243-5.406]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[5.356-5.507]</c:v>
+                  <c:v>[5.406-5.57]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[5.507-5.659]</c:v>
+                  <c:v>[5.57-5.733]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[5.659-5.811]</c:v>
+                  <c:v>[5.733-5.897]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[5.811-5.963]</c:v>
+                  <c:v>[5.897-6.06]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[5.963-6.115]</c:v>
+                  <c:v>[6.06-6.224]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3029,43 +3029,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>23</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>3</c:v>
@@ -3205,46 +3205,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[4.157-4.27]</c:v>
+                  <c:v>[4.142-4.277]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[4.27-4.383]</c:v>
+                  <c:v>[4.277-4.412]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[4.383-4.496]</c:v>
+                  <c:v>[4.412-4.546]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[4.496-4.608]</c:v>
+                  <c:v>[4.546-4.681]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[4.608-4.721]</c:v>
+                  <c:v>[4.681-4.816]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[4.721-4.834]</c:v>
+                  <c:v>[4.816-4.951]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[4.834-4.947]</c:v>
+                  <c:v>[4.951-5.086]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[4.947-5.059]</c:v>
+                  <c:v>[5.086-5.221]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[5.059-5.172]</c:v>
+                  <c:v>[5.221-5.356]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[5.172-5.285]</c:v>
+                  <c:v>[5.356-5.491]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[5.285-5.398]</c:v>
+                  <c:v>[5.491-5.626]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[5.398-5.51]</c:v>
+                  <c:v>[5.626-5.761]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[5.51-5.623]</c:v>
+                  <c:v>[5.761-5.896]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[5.623-5.736]</c:v>
+                  <c:v>[5.896-6.031]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3259,43 +3259,43 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3432,46 +3432,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[4.469-4.587]</c:v>
+                  <c:v>[4.299-4.437]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[4.587-4.704]</c:v>
+                  <c:v>[4.437-4.574]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[4.704-4.822]</c:v>
+                  <c:v>[4.574-4.711]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[4.822-4.939]</c:v>
+                  <c:v>[4.711-4.849]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[4.939-5.057]</c:v>
+                  <c:v>[4.849-4.986]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[5.057-5.174]</c:v>
+                  <c:v>[4.986-5.124]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[5.174-5.292]</c:v>
+                  <c:v>[5.124-5.261]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[5.292-5.409]</c:v>
+                  <c:v>[5.261-5.399]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[5.409-5.527]</c:v>
+                  <c:v>[5.399-5.536]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[5.527-5.644]</c:v>
+                  <c:v>[5.536-5.674]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[5.644-5.762]</c:v>
+                  <c:v>[5.674-5.811]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[5.762-5.88]</c:v>
+                  <c:v>[5.811-5.949]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[5.88-5.997]</c:v>
+                  <c:v>[5.949-6.086]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[5.997-6.115]</c:v>
+                  <c:v>[6.086-6.224]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3483,46 +3483,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="6">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3659,46 +3659,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.99-4.113]</c:v>
+                  <c:v>[3.935-4.044]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[4.113-4.236]</c:v>
+                  <c:v>[4.044-4.154]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[4.236-4.359]</c:v>
+                  <c:v>[4.154-4.263]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[4.359-4.483]</c:v>
+                  <c:v>[4.263-4.373]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[4.483-4.606]</c:v>
+                  <c:v>[4.373-4.483]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[4.606-4.729]</c:v>
+                  <c:v>[4.483-4.592]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[4.729-4.852]</c:v>
+                  <c:v>[4.592-4.702]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[4.852-4.976]</c:v>
+                  <c:v>[4.702-4.811]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[4.976-5.099]</c:v>
+                  <c:v>[4.811-4.921]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[5.099-5.222]</c:v>
+                  <c:v>[4.921-5.03]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[5.222-5.345]</c:v>
+                  <c:v>[5.03-5.14]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[5.345-5.469]</c:v>
+                  <c:v>[5.14-5.249]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[5.469-5.592]</c:v>
+                  <c:v>[5.249-5.359]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[5.592-5.715]</c:v>
+                  <c:v>[5.359-5.468]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3710,46 +3710,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3886,46 +3886,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[8.22-8.48]</c:v>
+                  <c:v>[8.02-8.31]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[8.48-8.74]</c:v>
+                  <c:v>[8.31-8.59]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[8.74-9.0]</c:v>
+                  <c:v>[8.59-8.87]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[9.0-9.26]</c:v>
+                  <c:v>[8.87-9.15]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[9.26-9.53]</c:v>
+                  <c:v>[9.15-9.44]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[9.53-9.79]</c:v>
+                  <c:v>[9.44-9.72]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[9.79-10.05]</c:v>
+                  <c:v>[9.72-10.0]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[10.05-10.31]</c:v>
+                  <c:v>[10.0-10.28]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[10.31-10.57]</c:v>
+                  <c:v>[10.28-10.56]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[10.57-10.83]</c:v>
+                  <c:v>[10.56-10.85]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[10.83-11.09]</c:v>
+                  <c:v>[10.85-11.13]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[11.09-11.36]</c:v>
+                  <c:v>[11.13-11.41]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[11.36-11.62]</c:v>
+                  <c:v>[11.41-11.69]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[11.62-11.88]</c:v>
+                  <c:v>[11.69-11.98]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3937,46 +3937,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>46</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4929,7 +4929,7 @@
         <v>8</v>
       </c>
       <c r="B1">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4937,7 +4937,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4945,7 +4945,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>109</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4953,7 +4953,7 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4961,7 +4961,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4969,7 +4969,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4977,7 +4977,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>31</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5020,7 +5020,7 @@
         <v>70</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5028,7 +5028,7 @@
         <v>71</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5036,7 +5036,7 @@
         <v>72</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5044,7 +5044,7 @@
         <v>73</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5052,7 +5052,7 @@
         <v>74</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5060,7 +5060,7 @@
         <v>75</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5068,7 +5068,7 @@
         <v>76</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5076,7 +5076,7 @@
         <v>77</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5084,7 +5084,7 @@
         <v>78</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5092,7 +5092,7 @@
         <v>79</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5100,7 +5100,7 @@
         <v>80</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5108,7 +5108,7 @@
         <v>81</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5116,7 +5116,7 @@
         <v>82</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5124,7 +5124,7 @@
         <v>83</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5154,7 +5154,7 @@
         <v>85</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5162,7 +5162,7 @@
         <v>86</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5170,7 +5170,7 @@
         <v>87</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5178,7 +5178,7 @@
         <v>88</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5186,7 +5186,7 @@
         <v>89</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5194,7 +5194,7 @@
         <v>90</v>
       </c>
       <c r="B7">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5202,7 +5202,7 @@
         <v>91</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5210,7 +5210,7 @@
         <v>92</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5226,7 +5226,7 @@
         <v>94</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5234,7 +5234,7 @@
         <v>95</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5242,7 +5242,7 @@
         <v>96</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5250,7 +5250,7 @@
         <v>97</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5272,7 +5272,7 @@
         <v>98</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5280,7 +5280,7 @@
         <v>99</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5288,7 +5288,7 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5296,7 +5296,7 @@
         <v>101</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5304,7 +5304,7 @@
         <v>102</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5312,7 +5312,7 @@
         <v>103</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5320,7 +5320,7 @@
         <v>104</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5336,7 +5336,7 @@
         <v>106</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5344,7 +5344,7 @@
         <v>107</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5352,7 +5352,7 @@
         <v>108</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5360,7 +5360,7 @@
         <v>109</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5368,7 +5368,7 @@
         <v>110</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5376,7 +5376,7 @@
         <v>111</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5406,7 +5406,7 @@
         <v>113</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5414,7 +5414,7 @@
         <v>114</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5422,7 +5422,7 @@
         <v>115</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5430,7 +5430,7 @@
         <v>116</v>
       </c>
       <c r="B5">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5438,7 +5438,7 @@
         <v>117</v>
       </c>
       <c r="B6">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5446,7 +5446,7 @@
         <v>118</v>
       </c>
       <c r="B7">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5454,7 +5454,7 @@
         <v>119</v>
       </c>
       <c r="B8">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5462,7 +5462,7 @@
         <v>120</v>
       </c>
       <c r="B9">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5470,7 +5470,7 @@
         <v>121</v>
       </c>
       <c r="B10">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5478,7 +5478,7 @@
         <v>122</v>
       </c>
       <c r="B11">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5486,7 +5486,7 @@
         <v>123</v>
       </c>
       <c r="B12">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5494,7 +5494,7 @@
         <v>124</v>
       </c>
       <c r="B13">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5502,7 +5502,7 @@
         <v>125</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5524,7 +5524,7 @@
         <v>126</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5532,7 +5532,7 @@
         <v>127</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5540,7 +5540,7 @@
         <v>128</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5556,7 +5556,7 @@
         <v>130</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5564,7 +5564,7 @@
         <v>131</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5588,7 +5588,7 @@
         <v>134</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5596,7 +5596,7 @@
         <v>135</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5604,7 +5604,7 @@
         <v>136</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5612,7 +5612,7 @@
         <v>137</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5628,7 +5628,7 @@
         <v>139</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -5650,7 +5650,7 @@
         <v>140</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5658,7 +5658,7 @@
         <v>141</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5666,7 +5666,7 @@
         <v>142</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5674,7 +5674,7 @@
         <v>143</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5682,7 +5682,7 @@
         <v>144</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5690,7 +5690,7 @@
         <v>145</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5698,7 +5698,7 @@
         <v>146</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5706,7 +5706,7 @@
         <v>147</v>
       </c>
       <c r="B8">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5714,7 +5714,7 @@
         <v>148</v>
       </c>
       <c r="B9">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5722,7 +5722,7 @@
         <v>149</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5738,7 +5738,7 @@
         <v>151</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5746,7 +5746,7 @@
         <v>152</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5754,7 +5754,7 @@
         <v>153</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5776,7 +5776,7 @@
         <v>154</v>
       </c>
       <c r="B1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5784,7 +5784,7 @@
         <v>155</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5792,7 +5792,7 @@
         <v>156</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5800,7 +5800,7 @@
         <v>157</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5808,7 +5808,7 @@
         <v>158</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5816,7 +5816,7 @@
         <v>159</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5824,7 +5824,7 @@
         <v>160</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5832,7 +5832,7 @@
         <v>161</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5840,7 +5840,7 @@
         <v>162</v>
       </c>
       <c r="B9">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5848,7 +5848,7 @@
         <v>163</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5856,7 +5856,7 @@
         <v>164</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5864,7 +5864,7 @@
         <v>165</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5872,7 +5872,7 @@
         <v>166</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5902,7 +5902,7 @@
         <v>8</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5910,7 +5910,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5918,7 +5918,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5926,15 +5926,15 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5942,20 +5942,20 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -5963,15 +5963,15 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -6001,7 +6001,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6009,7 +6009,7 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6017,7 +6017,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6025,7 +6025,7 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6049,7 +6049,7 @@
         <v>17</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6057,7 +6057,7 @@
         <v>18</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6084,7 +6084,7 @@
         <v>8</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6092,7 +6092,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6108,7 +6108,7 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6116,7 +6116,7 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6124,7 +6124,7 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6132,7 +6132,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6148,7 +6148,7 @@
         <v>21</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6175,7 +6175,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6191,7 +6191,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6199,7 +6199,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6207,7 +6207,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6215,7 +6215,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6223,7 +6223,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6231,7 +6231,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6239,7 +6239,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6247,7 +6247,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6255,7 +6255,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6263,7 +6263,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6271,7 +6271,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6309,7 +6309,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6317,7 +6317,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6325,7 +6325,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6333,7 +6333,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6341,7 +6341,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6349,7 +6349,7 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6357,7 +6357,7 @@
         <v>21</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6365,7 +6365,7 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6373,7 +6373,7 @@
         <v>23</v>
       </c>
       <c r="B10">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6381,7 +6381,7 @@
         <v>24</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6389,7 +6389,7 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6405,7 +6405,7 @@
         <v>27</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6427,7 +6427,7 @@
         <v>28</v>
       </c>
       <c r="B1">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6435,7 +6435,7 @@
         <v>29</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6443,7 +6443,7 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6451,7 +6451,7 @@
         <v>31</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6459,7 +6459,7 @@
         <v>32</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6467,7 +6467,7 @@
         <v>33</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6475,7 +6475,7 @@
         <v>34</v>
       </c>
       <c r="B7">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6483,7 +6483,7 @@
         <v>35</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6491,7 +6491,7 @@
         <v>36</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6499,7 +6499,7 @@
         <v>37</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6507,7 +6507,7 @@
         <v>38</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6515,7 +6515,7 @@
         <v>39</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6531,7 +6531,7 @@
         <v>41</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -6553,7 +6553,7 @@
         <v>42</v>
       </c>
       <c r="B1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6561,7 +6561,7 @@
         <v>43</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6569,7 +6569,7 @@
         <v>44</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6585,7 +6585,7 @@
         <v>46</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6593,7 +6593,7 @@
         <v>47</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6609,7 +6609,7 @@
         <v>49</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6617,7 +6617,7 @@
         <v>50</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6625,7 +6625,7 @@
         <v>51</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6633,7 +6633,7 @@
         <v>52</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6641,7 +6641,7 @@
         <v>53</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6649,7 +6649,7 @@
         <v>54</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6657,7 +6657,7 @@
         <v>55</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6679,7 +6679,7 @@
         <v>56</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6687,7 +6687,7 @@
         <v>57</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6695,7 +6695,7 @@
         <v>58</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6703,7 +6703,7 @@
         <v>59</v>
       </c>
       <c r="B4">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6711,7 +6711,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6719,7 +6719,7 @@
         <v>61</v>
       </c>
       <c r="B6">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6727,7 +6727,7 @@
         <v>62</v>
       </c>
       <c r="B7">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6735,7 +6735,7 @@
         <v>63</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6743,7 +6743,7 @@
         <v>64</v>
       </c>
       <c r="B9">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6751,7 +6751,7 @@
         <v>65</v>
       </c>
       <c r="B10">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6759,7 +6759,7 @@
         <v>66</v>
       </c>
       <c r="B11">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6767,7 +6767,7 @@
         <v>67</v>
       </c>
       <c r="B12">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6775,7 +6775,7 @@
         <v>68</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6783,7 +6783,7 @@
         <v>69</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>